<commit_message>
Add Group Access for Insert / Update
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RoyalPetz---WORKING-Copy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_PROJECT_\RoyalPetz - WORKING Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>MANAJEMEN USER</t>
   </si>
@@ -41,12 +41,6 @@
     <t>TAMBAH / UPDATE MUTASI BARANG</t>
   </si>
   <si>
-    <t>PENERIMAAN BARANG DARI MUTASI</t>
-  </si>
-  <si>
-    <t>PENERIMAAN BARANG DARI PO</t>
-  </si>
-  <si>
     <t>REQUEST ORDER</t>
   </si>
   <si>
@@ -90,6 +84,12 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>EXPORT</t>
+  </si>
+  <si>
+    <t>Auto add Transaksi Harian</t>
   </si>
 </sst>
 </file>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:G24"/>
+  <dimension ref="B4:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +418,7 @@
     <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -426,10 +426,10 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>1</v>
       </c>
@@ -437,10 +437,10 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>2</v>
       </c>
@@ -448,10 +448,10 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>3</v>
       </c>
@@ -459,106 +459,124 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>14</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>15</v>
       </c>
       <c r="E19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>16</v>
       </c>
@@ -566,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>17</v>
       </c>
@@ -574,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>18</v>
       </c>
@@ -582,20 +600,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>